<commit_message>
[Omkar] Add POM Freameworks selenium codes
</commit_message>
<xml_diff>
--- a/src/main/resources/repository/LoginTestData.xlsx
+++ b/src/main/resources/repository/LoginTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OMKAR BADE\IdeaProjects\POM_Framework\src\main\resources\repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9BA400E-08B8-4B61-A553-5A95BEB9F456}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F235CB3-8245-4EC9-A786-74B7C3C5D74D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="8964" xr2:uid="{E1E08A7C-24DA-4721-A174-11DF032E8F0D}"/>
+    <workbookView xWindow="1440" yWindow="2352" windowWidth="17280" windowHeight="8964" xr2:uid="{E1E08A7C-24DA-4721-A174-11DF032E8F0D}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
@@ -405,7 +405,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -427,7 +427,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -435,7 +435,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>